<commit_message>
most of the updates
</commit_message>
<xml_diff>
--- a/forms/thomas_form.xlsx
+++ b/forms/thomas_form.xlsx
@@ -6948,10 +6948,10 @@
   <dimension ref="A1:BU948"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="6" topLeftCell="BP7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="6" topLeftCell="AJ7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="BQ6" sqref="BQ6"/>
+      <selection pane="bottomRight" activeCell="AS5" sqref="AS5:AS6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>

</xml_diff>